<commit_message>
Updated resources for material and amino acid data
</commit_message>
<xml_diff>
--- a/MorbidJava/resources/data/AminoAcid.xlsx
+++ b/MorbidJava/resources/data/AminoAcid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15945" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">colors!$A$1:$I$21</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -630,6 +631,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -646,7 +715,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F8F4D6"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -928,10 +997,14 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>